<commit_message>
Made some loading time changes
Added code in the run file to help improve upon the page load times
</commit_message>
<xml_diff>
--- a/application/static/data/Data in sectors as of 8th September 2020.xlsx
+++ b/application/static/data/Data in sectors as of 8th September 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barlowkasule/Desktop/infinity/application/static/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5683F3-3885-3B49-BA3F-C55F7F5C336B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF8159A-74D4-0743-8486-3AFFAE003FDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="440" windowWidth="24000" windowHeight="9740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accountability sector " sheetId="1" r:id="rId1"/>
@@ -4043,8 +4043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="F185" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="G169" sqref="G169:G171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4053,7 +4053,7 @@
     <col min="2" max="2" width="24.33203125" style="27" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" style="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="27"/>
+    <col min="5" max="5" width="16.33203125" style="27" customWidth="1"/>
     <col min="6" max="6" width="12" style="27" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.83203125" style="27"/>
   </cols>

</xml_diff>